<commit_message>
cambio formato hora cinemas
</commit_message>
<xml_diff>
--- a/Script/cinemas - 26-08-2022.xlsx
+++ b/Script/cinemas - 26-08-2022.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>02:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>05:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>02:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>05:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>07:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -648,12 +648,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>08:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>01:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>07:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>02:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -808,12 +808,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>04:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>06:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>08:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -904,12 +904,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ESCALERA AL INFIERNO</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>06:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ESCALERA AL INFIERNO</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>08:25 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=6, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -968,12 +968,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>12:50 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1000,12 +1000,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>ESCALERA AL INFIERNO</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>03:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=6, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1032,12 +1032,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>ESCALERA AL INFIERNO</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>05:40 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=25, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>08:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=50, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1096,12 +1096,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>DC LIGA DE SUPER MASCOTAS</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>02:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1128,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>DC LIGA DE SUPER MASCOTAS</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>04:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=40, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1160,12 +1160,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>EL TELÉFONO NEGRO</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>01:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1192,12 +1192,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>EL TELÉFONO NEGRO</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>06:40 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1224,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>EL TELÉFONO NEGRO</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>08:35 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1256,12 +1256,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ELVIS</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1288,12 +1288,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ELVIS</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>07:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1320,12 +1320,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>THOR: AMOR Y TRUENO</t>
+          <t>TOP GUN: MAVERICK</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>01:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=55, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1352,12 +1352,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>THOR: AMOR Y TRUENO</t>
+          <t>TOP GUN: MAVERICK</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>04:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1384,12 +1384,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>THOR: AMOR Y TRUENO</t>
+          <t>TOP GUN: MAVERICK</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>07:40 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>01:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1443,17 +1443,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>03:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1475,17 +1475,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>05:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1507,17 +1507,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>TOP GUN: MAVERICK</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>12:55 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1539,17 +1539,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TOP GUN: MAVERICK</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>04:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1571,17 +1571,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GALERÍAS</t>
+          <t>PLAZA INTER</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>TOP GUN: MAVERICK</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>07:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=50, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1608,12 +1608,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>04:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=40, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1640,12 +1640,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>05:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1672,12 +1672,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>07:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>02:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1736,12 +1736,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>04:50 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1768,12 +1768,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>07:40 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1800,12 +1800,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>01:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1832,12 +1832,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>03:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1864,12 +1864,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>DC LIGA DE SUPER MASCOTAS</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>05:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=40, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>07:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1928,12 +1928,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>01:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1960,12 +1960,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>07:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -1987,17 +1987,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>PLAZA INTER</t>
+          <t>BELLO HORIZONTE</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>01:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2019,17 +2019,17 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>PLAZA INTER</t>
+          <t>BELLO HORIZONTE</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>12:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>03:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2120,12 +2120,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>05:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=10, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2152,12 +2152,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>08:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>01:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>04:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=45, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2248,12 +2248,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>07:45 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>01:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>03:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>05:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>07:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>06:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=6, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>08:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>05:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>05:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>08:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2600,12 +2600,12 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>DC LIGA DE SUPER MASCOTAS</t>
+          <t>TREN BALA</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>01:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=8, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>03:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2664,12 +2664,12 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>THOR: AMOR Y TRUENO</t>
+          <t>DC LIGA DE SUPER MASCOTAS</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>07:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2696,12 +2696,12 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>DC LIGA DE SUPER MASCOTAS</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>12:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2728,12 +2728,12 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>THOR: AMOR Y TRUENO</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>02:30 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>04:25 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=10, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2787,17 +2787,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>MASAYA</t>
+          <t>BELLO HORIZONTE</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>05:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2819,17 +2819,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>MASAYA</t>
+          <t>BELLO HORIZONTE</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>AFTER: AMOR INFINITO</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>07:55 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=30, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2851,17 +2851,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>MASAYA</t>
+          <t>BELLO HORIZONTE</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>02:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=25, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2888,12 +2888,12 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>04:50 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>NOPE</t>
+          <t>AFTER: AMOR INFINITO</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>07:40 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=55, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2952,12 +2952,12 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>01:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -2984,12 +2984,12 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3016,12 +3016,12 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>05:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=50, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3048,12 +3048,12 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>DRAGON BALL SUPER: SUPER HERO</t>
+          <t>NOPE</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>07:00 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=40, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>04:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3112,12 +3112,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>TREN BALA</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>07:15 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3144,12 +3144,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>DC LIGA DE SUPER MASCOTAS</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>02:10 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3176,12 +3176,12 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>MINIONS: NACE UN VILLANO</t>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>01:20 PM</t>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=5, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>
@@ -3208,12 +3208,236 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
+          <t>DRAGON BALL SUPER: SUPER HERO</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>TREN BALA</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=4, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>TREN BALA</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=7, tm_min=15, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>DC LIGA DE SUPER MASCOTAS</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=12, tm_min=0, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>DC LIGA DE SUPER MASCOTAS</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=2, tm_min=10, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
           <t>MINIONS: NACE UN VILLANO</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>03:20 PM</t>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=11, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>MINIONS: NACE UN VILLANO</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=1, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>26-08-2022</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Cinemas</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>MASAYA</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>MINIONS: NACE UN VILLANO</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>time.struct_time(tm_year=1900, tm_mon=1, tm_mday=1, tm_hour=3, tm_min=20, tm_sec=0, tm_wday=0, tm_yday=1, tm_isdst=-1)</t>
         </is>
       </c>
     </row>

</xml_diff>